<commit_message>
in progress for europe 30sec
</commit_message>
<xml_diff>
--- a/config/30sec_europe/parallelization_strategy.xlsx
+++ b/config/30sec_europe/parallelization_strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\edwin\github\edwinkost\PCR-GLOBWB_model_edwin-private-development\config\30sec_europe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37E5C1F9-3D5B-4F16-BF6C-CF1FAF2AEA5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB1A1A-FD16-46D9-B5EE-3589C39D4751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-6045" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{4EC1BA9B-84D7-48C9-B6D4-2077D303DA96}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="51">
   <si>
     <t>mask_10.map</t>
   </si>
@@ -172,16 +172,40 @@
   </si>
   <si>
     <t>mask_9.map</t>
+  </si>
+  <si>
+    <t>030000</t>
+  </si>
+  <si>
+    <t>job_nr</t>
+  </si>
+  <si>
+    <t>clone_1</t>
+  </si>
+  <si>
+    <t>clone_2</t>
+  </si>
+  <si>
+    <t>clone_3</t>
+  </si>
+  <si>
+    <t>cores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,8 +231,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,598 +1096,1541 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8D895E-0F63-4CFD-97E4-DC7793DC9C17}">
-  <dimension ref="B1:E45"/>
+  <dimension ref="B1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>4968256</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D1">
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E1">
-        <f>SUM(B1)</f>
+      <c r="F2">
+        <f>SUM(B2)</f>
         <v>4968256</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2">
+        <f>IF(E2=E1,"",E2)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <f>IF(E2=E1,"",D2)</f>
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="str">
+        <f>IF(E3=E2,D3,"")</f>
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(E4=E2,D4,"")</f>
+        <v/>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="2" t="str">
+        <f>LEFT(T2,2)</f>
+        <v>03</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>3643456</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E2">
-        <f>SUM(B2)</f>
+      <c r="F3">
+        <f>SUM(B3)</f>
         <v>3643456</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="H3">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I46" si="0">IF(E3=E2,"",E3)</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J46" si="1">IF(E3=E2,"",D3)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f>IF(E4=E3,D4,"")</f>
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L46" si="2">IF(E5=E3,D5,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>3456256</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="2">
+        <v>13</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E3">
-        <f>SUM(B3)</f>
+      <c r="F4">
+        <f>SUM(B4)</f>
         <v>3456256</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="H4">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>IF(E5=E4,D5,"")</f>
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>3024256</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="E4">
-        <f>SUM(B4)</f>
+      <c r="F5">
+        <f>SUM(B5)</f>
         <v>3024256</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="H5">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f>IF(E6=E5,D6,"")</f>
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>2822656</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="2">
+        <v>30</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K6" s="2">
+        <f>IF(E7=E6,D7,"")</f>
+        <v>25</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>115456</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="2">
+        <v>25</v>
+      </c>
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="E6">
-        <f>SUM(B5:B6)</f>
+      <c r="F7">
+        <f>SUM(B6:B7)</f>
         <v>2938112</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K7" s="2" t="str">
+        <f>IF(E8=E7,D8,"")</f>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>2765056</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="2">
+        <v>19</v>
+      </c>
+      <c r="E8">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="K8" s="2">
+        <f>IF(E9=E8,D9,"")</f>
+        <v>36</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>216256</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="2">
+        <v>36</v>
+      </c>
+      <c r="E9">
         <v>6</v>
       </c>
-      <c r="E8">
-        <f>SUM(B7:B8)</f>
+      <c r="F9">
+        <f>SUM(B8:B9)</f>
         <v>2981312</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K9" s="2" t="str">
+        <f>IF(E10=E9,D10,"")</f>
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>2765056</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K10" s="2">
+        <f>IF(E11=E10,D11,"")</f>
+        <v>22</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>230656</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D10">
+      <c r="D11" s="2">
+        <v>22</v>
+      </c>
+      <c r="E11">
         <v>7</v>
       </c>
-      <c r="E10">
-        <f>SUM(B9:B10)</f>
+      <c r="F11">
+        <f>SUM(B10:B11)</f>
         <v>2995712</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K11" s="2" t="str">
+        <f>IF(E12=E11,D12,"")</f>
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>2448256</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="2">
+        <v>39</v>
+      </c>
+      <c r="E12">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="K12" s="2">
+        <f>IF(E13=E12,D13,"")</f>
+        <v>2</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>302656</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D12">
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13">
         <v>8</v>
       </c>
-      <c r="E12">
-        <f>SUM(B11:B12)</f>
+      <c r="F13">
+        <f>SUM(B12:B13)</f>
         <v>2750912</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K13" s="2" t="str">
+        <f>IF(E14=E13,D14,"")</f>
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>1872256</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="2">
+        <v>44</v>
+      </c>
+      <c r="E14">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="K14" s="2">
+        <f>IF(E15=E14,D15,"")</f>
+        <v>14</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>302656</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15">
         <v>9</v>
       </c>
-      <c r="E14">
-        <f>SUM(B13:B14)</f>
+      <c r="F15">
+        <f>SUM(B14:B15)</f>
         <v>2174912</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K15" s="2" t="str">
+        <f>IF(E16=E15,D16,"")</f>
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16">
         <v>1843456</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="2">
+        <v>23</v>
+      </c>
+      <c r="E16">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="K16" s="2">
+        <f>IF(E17=E16,D17,"")</f>
+        <v>16</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
         <v>345856</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17">
         <v>10</v>
       </c>
-      <c r="E16">
-        <f>SUM(B15:B16)</f>
+      <c r="F17">
+        <f>SUM(B16:B17)</f>
         <v>2189312</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="I17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K17" s="2" t="str">
+        <f>IF(E18=E17,D18,"")</f>
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18">
         <v>1814656</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="2">
+        <v>34</v>
+      </c>
+      <c r="E18">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="H18">
+        <v>12</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K18" s="2">
+        <f>IF(E19=E18,D19,"")</f>
+        <v>5</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>403456</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19">
         <v>11</v>
       </c>
-      <c r="E18">
-        <f>SUM(B17:B18)</f>
+      <c r="F19">
+        <f>SUM(B18:B19)</f>
         <v>2218112</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K19" s="2" t="str">
+        <f>IF(E20=E19,D20,"")</f>
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20">
         <v>1411456</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="2">
+        <v>18</v>
+      </c>
+      <c r="E20">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="K20" s="2">
+        <f>IF(E21=E20,D21,"")</f>
+        <v>40</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21">
         <v>1109056</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="D20">
+      <c r="D21" s="2">
+        <v>40</v>
+      </c>
+      <c r="E21">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K21" s="2">
+        <f>IF(E22=E21,D22,"")</f>
+        <v>38</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22">
         <v>403456</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="2">
+        <v>38</v>
+      </c>
+      <c r="E22">
         <v>12</v>
       </c>
-      <c r="E21">
-        <f>SUM(B19:B21)</f>
+      <c r="F22">
+        <f>SUM(B20:B22)</f>
         <v>2923968</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K22" s="2" t="str">
+        <f>IF(E23=E22,D23,"")</f>
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>1382656</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="D22">
+      <c r="D23" s="2">
+        <v>33</v>
+      </c>
+      <c r="E23">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="K23" s="2">
+        <f>IF(E24=E23,D24,"")</f>
+        <v>9</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>1109056</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="D23">
+      <c r="D24" s="2">
+        <v>9</v>
+      </c>
+      <c r="E24">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K24" s="2">
+        <f>IF(E25=E24,D25,"")</f>
+        <v>29</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>432256</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="D24">
+      <c r="D25" s="2">
+        <v>29</v>
+      </c>
+      <c r="E25">
         <v>13</v>
       </c>
-      <c r="E24">
-        <f>SUM(B22:B24)</f>
+      <c r="F25">
+        <f>SUM(B23:B25)</f>
         <v>2923968</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K25" s="2" t="str">
+        <f>IF(E26=E25,D26,"")</f>
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>1296256</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>2</v>
       </c>
-      <c r="D25">
+      <c r="D26" s="2">
+        <v>12</v>
+      </c>
+      <c r="E26">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K26" s="2">
+        <f>IF(E27=E26,D27,"")</f>
+        <v>20</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27">
         <v>1008256</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>11</v>
       </c>
-      <c r="D26">
+      <c r="D27" s="2">
+        <v>20</v>
+      </c>
+      <c r="E27">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K27" s="2">
+        <f>IF(E28=E27,D28,"")</f>
+        <v>43</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28">
         <v>504256</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="D27">
+      <c r="D28" s="2">
+        <v>43</v>
+      </c>
+      <c r="E28">
         <v>14</v>
       </c>
-      <c r="E27">
-        <f>SUM(B25:B27)</f>
+      <c r="F28">
+        <f>SUM(B26:B28)</f>
         <v>2808768</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J28" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K28" s="2" t="str">
+        <f>IF(E29=E28,D29,"")</f>
+        <v/>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29">
         <v>1296256</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>17</v>
       </c>
-      <c r="D28">
+      <c r="D29" s="2">
+        <v>26</v>
+      </c>
+      <c r="E29">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="H29">
+        <v>8</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="K29" s="2">
+        <f>IF(E30=E29,D30,"")</f>
+        <v>27</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30">
         <v>1008256</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>18</v>
       </c>
-      <c r="D29">
+      <c r="D30" s="2">
+        <v>27</v>
+      </c>
+      <c r="E30">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30">
+      <c r="I30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J30" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K30" s="2">
+        <f>IF(E31=E30,D31,"")</f>
+        <v>31</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31">
         <v>518656</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>23</v>
       </c>
-      <c r="D30">
+      <c r="D31" s="2">
+        <v>31</v>
+      </c>
+      <c r="E31">
         <v>15</v>
       </c>
-      <c r="E30">
-        <f>SUM(B28:B30)</f>
+      <c r="F31">
+        <f>SUM(B29:B31)</f>
         <v>2823168</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J31" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K31" s="2" t="str">
+        <f>IF(E32=E31,D32,"")</f>
+        <v/>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32">
         <v>1267456</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>29</v>
       </c>
-      <c r="D31">
+      <c r="D32" s="2">
+        <v>37</v>
+      </c>
+      <c r="E32">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32">
+      <c r="H32">
+        <v>8</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="K32" s="2">
+        <f>IF(E33=E32,D33,"")</f>
+        <v>17</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33">
         <v>907456</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>7</v>
       </c>
-      <c r="D32">
+      <c r="D33" s="2">
+        <v>17</v>
+      </c>
+      <c r="E33">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33">
+      <c r="I33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K33" s="2">
+        <f>IF(E34=E33,D34,"")</f>
+        <v>24</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34">
         <v>518656</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>15</v>
       </c>
-      <c r="D33">
+      <c r="D34" s="2">
+        <v>24</v>
+      </c>
+      <c r="E34">
         <v>16</v>
       </c>
-      <c r="E33">
-        <f>SUM(B31:B33)</f>
+      <c r="F34">
+        <f>SUM(B32:B34)</f>
         <v>2693568</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K34" s="2" t="str">
+        <f>IF(E35=E34,D35,"")</f>
+        <v/>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35">
         <v>1209856</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>42</v>
       </c>
-      <c r="D34">
+      <c r="D35" s="2">
+        <v>7</v>
+      </c>
+      <c r="E35">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35">
+      <c r="H35">
+        <v>8</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K35" s="2">
+        <f>IF(E36=E35,D36,"")</f>
+        <v>45</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36">
         <v>907456</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="D35">
+      <c r="D36" s="2">
+        <v>45</v>
+      </c>
+      <c r="E36">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36">
+      <c r="I36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J36" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K36" s="2">
+        <f>IF(E37=E36,D37,"")</f>
+        <v>42</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>605056</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>35</v>
       </c>
-      <c r="D36">
+      <c r="D37" s="2">
+        <v>42</v>
+      </c>
+      <c r="E37">
         <v>17</v>
       </c>
-      <c r="E36">
-        <f>SUM(B34:B36)</f>
+      <c r="F37">
+        <f>SUM(B35:B37)</f>
         <v>2722368</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37">
+      <c r="I37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K37" s="2" t="str">
+        <f>IF(E38=E37,D38,"")</f>
+        <v/>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>1209856</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>43</v>
       </c>
-      <c r="D37">
+      <c r="D38" s="2">
+        <v>8</v>
+      </c>
+      <c r="E38">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38">
+      <c r="H38">
+        <v>8</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K38" s="2">
+        <f>IF(E39=E38,D39,"")</f>
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>907456</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>39</v>
       </c>
-      <c r="D38">
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39">
+      <c r="I39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K39" s="2">
+        <f>IF(E40=E39,D40,"")</f>
+        <v>41</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40">
         <v>605056</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>34</v>
       </c>
-      <c r="D39">
+      <c r="D40" s="2">
+        <v>41</v>
+      </c>
+      <c r="E40">
         <v>18</v>
       </c>
-      <c r="E39">
-        <f>SUM(B37:B39)</f>
+      <c r="F40">
+        <f>SUM(B38:B40)</f>
         <v>2722368</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40">
+      <c r="I40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K40" s="2" t="str">
+        <f>IF(E41=E40,D41,"")</f>
+        <v/>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41">
         <v>1166656</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>5</v>
       </c>
-      <c r="D40">
+      <c r="D41" s="2">
+        <v>15</v>
+      </c>
+      <c r="E41">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41">
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="K41" s="2">
+        <f>IF(E42=E41,D42,"")</f>
+        <v>21</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42">
         <v>864256</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>12</v>
       </c>
-      <c r="D41">
+      <c r="D42" s="2">
+        <v>21</v>
+      </c>
+      <c r="E42">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42">
+      <c r="I42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K42" s="2">
+        <f>IF(E43=E42,D43,"")</f>
+        <v>28</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>605056</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>19</v>
       </c>
-      <c r="D42">
+      <c r="D43" s="2">
+        <v>28</v>
+      </c>
+      <c r="E43">
         <v>19</v>
       </c>
-      <c r="E42">
-        <f>SUM(B40:B42)</f>
+      <c r="F43">
+        <f>SUM(B41:B43)</f>
         <v>2635968</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43">
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K43" s="2" t="str">
+        <f>IF(E44=E43,D44,"")</f>
+        <v/>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44">
         <v>1152256</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>1</v>
       </c>
-      <c r="D43">
+      <c r="D44" s="2">
+        <v>11</v>
+      </c>
+      <c r="E44">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44">
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="K44" s="2">
+        <f>IF(E45=E44,D45,"")</f>
+        <v>32</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45">
         <v>864256</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>24</v>
       </c>
-      <c r="D44">
+      <c r="D45" s="2">
+        <v>32</v>
+      </c>
+      <c r="E45">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45">
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J45" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K45" s="2">
+        <f>IF(E46=E45,D46,"")</f>
+        <v>35</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46">
         <v>648256</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>27</v>
       </c>
-      <c r="D45">
+      <c r="D46" s="2">
+        <v>35</v>
+      </c>
+      <c r="E46">
         <v>20</v>
       </c>
-      <c r="E45">
-        <f>SUM(B43:B45)</f>
+      <c r="F46">
+        <f>SUM(B44:B46)</f>
         <v>2664768</v>
       </c>
+      <c r="I46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J46" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K46" s="2" t="str">
+        <f>IF(E47=E46,D47,"")</f>
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:D45">
-    <sortCondition ref="D1:D45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E46">
+    <sortCondition ref="E2:E46"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>